<commit_message>
Corrected section 3199J1-04 in arabic and ls excel spreadsheet
</commit_message>
<xml_diff>
--- a/runs/constraint_files/Arabic and LS to Semesters.xlsx
+++ b/runs/constraint_files/Arabic and LS to Semesters.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/SarahGold/Documents/GitHub/scheduler/runs/constraint_files/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31CEEF92-8C2C-AE43-AB5E-A64638042DD7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="27795" windowHeight="14625" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="214">
   <si>
     <t>Sect ID</t>
   </si>
@@ -646,9 +652,6 @@
   </si>
   <si>
     <t>000116-05</t>
-  </si>
-  <si>
-    <t>3199J1-02</t>
   </si>
   <si>
     <t>3199J2-05</t>
@@ -666,7 +669,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -714,12 +717,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -961,6 +967,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1008,7 +1017,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1041,9 +1050,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1076,6 +1102,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1251,43 +1294,43 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="3.7109375" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.6640625" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="3" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.5" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="4" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="3.7109375" customWidth="1"/>
-    <col min="21" max="21" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="3.6640625" customWidth="1"/>
+    <col min="21" max="21" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="2" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="3" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="7" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.5" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="4" bestFit="1" customWidth="1"/>
     <col min="28" max="29" width="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1321,7 +1364,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1379,7 +1422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1461,7 +1504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -1543,7 +1586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -1625,7 +1668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>35</v>
       </c>
@@ -1707,7 +1750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -1780,7 +1823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -1865,7 +1908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>48</v>
       </c>
@@ -1947,7 +1990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>51</v>
       </c>
@@ -2029,7 +2072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>54</v>
       </c>
@@ -2111,7 +2154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>57</v>
       </c>
@@ -2193,7 +2236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>60</v>
       </c>
@@ -2275,7 +2318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -2357,7 +2400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>69</v>
       </c>
@@ -2439,7 +2482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>73</v>
       </c>
@@ -2521,7 +2564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -2606,7 +2649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>81</v>
       </c>
@@ -2688,7 +2731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>84</v>
       </c>
@@ -2770,7 +2813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>87</v>
       </c>
@@ -2852,7 +2895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>91</v>
       </c>
@@ -2934,7 +2977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>95</v>
       </c>
@@ -3016,7 +3059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>98</v>
       </c>
@@ -3101,7 +3144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>101</v>
       </c>
@@ -3183,7 +3226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>104</v>
       </c>
@@ -3265,7 +3308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>107</v>
       </c>
@@ -3347,7 +3390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>110</v>
       </c>
@@ -3550,39 +3593,40 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:W25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W1" sqref="W1:W1048576"/>
+      <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="2.7109375" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.6640625" customWidth="1"/>
+    <col min="11" max="11" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="3" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="7" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="3.85546875" customWidth="1"/>
-    <col min="18" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="3.83203125" customWidth="1"/>
+    <col min="18" max="18" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="2" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="3" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="7" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.5" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3619,7 +3663,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>116</v>
       </c>
@@ -3682,11 +3726,11 @@
       <c r="V2" t="s">
         <v>122</v>
       </c>
-      <c r="W2" t="s">
+      <c r="W2" s="5" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>123</v>
       </c>
@@ -3746,11 +3790,11 @@
       <c r="V3" t="s">
         <v>122</v>
       </c>
-      <c r="W3" t="s">
+      <c r="W3" s="5" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>127</v>
       </c>
@@ -3810,11 +3854,11 @@
       <c r="V4" t="s">
         <v>122</v>
       </c>
-      <c r="W4" t="s">
+      <c r="W4" s="5" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>131</v>
       </c>
@@ -3874,11 +3918,11 @@
       <c r="V5" t="s">
         <v>122</v>
       </c>
-      <c r="W5" t="s">
+      <c r="W5" s="5" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>134</v>
       </c>
@@ -3938,11 +3982,11 @@
       <c r="V6" t="s">
         <v>122</v>
       </c>
-      <c r="W6" t="s">
+      <c r="W6" s="5" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>137</v>
       </c>
@@ -4002,11 +4046,11 @@
       <c r="V7" t="s">
         <v>122</v>
       </c>
-      <c r="W7" t="s">
+      <c r="W7" s="5" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>140</v>
       </c>
@@ -4066,11 +4110,11 @@
       <c r="V8" t="s">
         <v>122</v>
       </c>
-      <c r="W8" t="s">
+      <c r="W8" s="5" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>143</v>
       </c>
@@ -4130,11 +4174,11 @@
       <c r="V9" t="s">
         <v>122</v>
       </c>
-      <c r="W9" t="s">
+      <c r="W9" s="5" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>146</v>
       </c>
@@ -4197,11 +4241,11 @@
       <c r="V10" t="s">
         <v>154</v>
       </c>
-      <c r="W10" t="s">
+      <c r="W10" s="5" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>155</v>
       </c>
@@ -4264,11 +4308,11 @@
       <c r="V11" t="s">
         <v>154</v>
       </c>
-      <c r="W11" t="s">
+      <c r="W11" s="5" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>158</v>
       </c>
@@ -4331,11 +4375,11 @@
       <c r="V12" t="s">
         <v>154</v>
       </c>
-      <c r="W12" t="s">
+      <c r="W12" s="5" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>161</v>
       </c>
@@ -4398,11 +4442,11 @@
       <c r="V13" t="s">
         <v>166</v>
       </c>
-      <c r="W13" t="s">
+      <c r="W13" s="5" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>167</v>
       </c>
@@ -4462,11 +4506,11 @@
       <c r="V14" t="s">
         <v>166</v>
       </c>
-      <c r="W14" t="s">
+      <c r="W14" s="5" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>170</v>
       </c>
@@ -4529,11 +4573,11 @@
       <c r="V15" t="s">
         <v>166</v>
       </c>
-      <c r="W15" t="s">
+      <c r="W15" s="5" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>173</v>
       </c>
@@ -4596,11 +4640,11 @@
       <c r="V16" t="s">
         <v>178</v>
       </c>
-      <c r="W16" t="s">
+      <c r="W16" s="5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>179</v>
       </c>
@@ -4663,11 +4707,11 @@
       <c r="V17" t="s">
         <v>178</v>
       </c>
-      <c r="W17" t="s">
+      <c r="W17" s="5" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>183</v>
       </c>
@@ -4730,11 +4774,11 @@
       <c r="V18" t="s">
         <v>178</v>
       </c>
-      <c r="W18" t="s">
+      <c r="W18" s="5" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>187</v>
       </c>
@@ -4797,11 +4841,11 @@
       <c r="V19" t="s">
         <v>178</v>
       </c>
-      <c r="W19" t="s">
+      <c r="W19" s="5" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>190</v>
       </c>
@@ -4864,11 +4908,11 @@
       <c r="V20" t="s">
         <v>178</v>
       </c>
-      <c r="W20" t="s">
+      <c r="W20" s="5" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>193</v>
       </c>
@@ -4931,11 +4975,11 @@
       <c r="V21" t="s">
         <v>201</v>
       </c>
-      <c r="W21" t="s">
+      <c r="W21" s="5" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>202</v>
       </c>
@@ -4998,11 +5042,11 @@
       <c r="V22" t="s">
         <v>198</v>
       </c>
-      <c r="W22" t="s">
+      <c r="W22" s="5" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>206</v>
       </c>
@@ -5065,11 +5109,11 @@
       <c r="V23" t="s">
         <v>201</v>
       </c>
-      <c r="W23" t="s">
+      <c r="W23" s="5" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>209</v>
       </c>
@@ -5099,7 +5143,7 @@
       </c>
       <c r="J24" s="1"/>
       <c r="K24" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="L24">
         <v>7</v>
@@ -5118,7 +5162,7 @@
       </c>
       <c r="Q24" s="1"/>
       <c r="R24" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="S24">
         <v>7</v>
@@ -5132,13 +5176,13 @@
       <c r="V24" t="s">
         <v>198</v>
       </c>
-      <c r="W24" t="s">
+      <c r="W24" s="5" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B25">
         <v>7</v>
@@ -5166,7 +5210,7 @@
       </c>
       <c r="J25" s="1"/>
       <c r="K25" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="L25">
         <v>7</v>
@@ -5185,7 +5229,7 @@
       </c>
       <c r="Q25" s="1"/>
       <c r="R25" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="S25">
         <v>7</v>
@@ -5199,7 +5243,7 @@
       <c r="V25" t="s">
         <v>201</v>
       </c>
-      <c r="W25" t="s">
+      <c r="W25" s="5" t="s">
         <v>147</v>
       </c>
     </row>
@@ -5209,12 +5253,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Made full_school_sections.py handle periods with two different team_3 classes properly
</commit_message>
<xml_diff>
--- a/runs/constraint_files/Arabic and LS to Semesters.xlsx
+++ b/runs/constraint_files/Arabic and LS to Semesters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/SarahGold/Documents/GitHub/scheduler/runs/constraint_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31CEEF92-8C2C-AE43-AB5E-A64638042DD7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC8BDCB9-DFC5-2249-9308-F450D7E40773}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="16140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="215">
   <si>
     <t>Sect ID</t>
   </si>
@@ -664,6 +664,9 @@
   </si>
   <si>
     <t>3199J1-04</t>
+  </si>
+  <si>
+    <t>3199J1-02</t>
   </si>
 </sst>
 </file>
@@ -3596,8 +3599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:W25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L35" sqref="L35"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5143,7 +5146,7 @@
       </c>
       <c r="J24" s="1"/>
       <c r="K24" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="L24">
         <v>7</v>

</xml_diff>